<commit_message>
add func DHT, NFR, EPC, APL_SIO, SP_CV + edit DB
</commit_message>
<xml_diff>
--- a/DB/raschet_turboagregata_predvaritelny.xlsx
+++ b/DB/raschet_turboagregata_predvaritelny.xlsx
@@ -35,11 +35,10 @@
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <vertAlign val="superscript"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -49,6 +48,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -113,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -139,16 +144,26 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -492,21 +507,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:K14"/>
+  <dimension ref="A2:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" ht="18" customHeight="1">
-      <c r="B2" s="9" t="inlineStr">
+      <c r="B2" s="15" t="inlineStr">
         <is>
           <t>Маркировка турбины</t>
         </is>
       </c>
-      <c r="C2" s="10" t="n"/>
+      <c r="C2" s="16" t="n"/>
       <c r="D2" s="2" t="inlineStr">
         <is>
           <t>N, МВт</t>
@@ -549,10 +564,18 @@
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="2" t="inlineStr"/>
-      <c r="C3" s="2" t="inlineStr"/>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Т-100-130</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>ЛМЗ, ЦВД</t>
+        </is>
+      </c>
       <c r="D3" s="3" t="n">
-        <v>213</v>
+        <v>0</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>13</v>
@@ -565,13 +588,13 @@
       </c>
       <c r="H3" s="3" t="n"/>
       <c r="I3" s="3" t="n">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>123</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5">
@@ -600,7 +623,7 @@
           <t>t, oC</t>
         </is>
       </c>
-      <c r="D8" s="9" t="inlineStr">
+      <c r="D8" s="15" t="inlineStr">
         <is>
           <t>h, кДж/кг</t>
         </is>
@@ -641,7 +664,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="11" t="inlineStr">
+      <c r="B11" s="9" t="inlineStr">
         <is>
           <t>1.2 Определение конечных параметров</t>
         </is>
@@ -659,7 +682,7 @@
           <t>t, oC</t>
         </is>
       </c>
-      <c r="D13" s="9" t="inlineStr">
+      <c r="D13" s="15" t="inlineStr">
         <is>
           <t>h, кДж/кг</t>
         </is>
@@ -685,7 +708,7 @@
         <f>G3</f>
         <v/>
       </c>
-      <c r="C14" s="12" t="n">
+      <c r="C14" s="10" t="n">
         <v>341.069773726435</v>
       </c>
       <c r="D14" s="6" t="n">
@@ -697,6 +720,196 @@
       </c>
       <c r="F14" s="8" t="n">
         <v>0.07308081411324667</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="9" t="inlineStr">
+        <is>
+          <t>1.3 Располагаемый теплоперепад</t>
+        </is>
+      </c>
+      <c r="C16" s="4" t="n"/>
+      <c r="D16" s="4" t="n"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="4" t="n"/>
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="4" t="n"/>
+    </row>
+    <row r="18" ht="18" customHeight="1">
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>H0=</t>
+        </is>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>390.7049863731177</v>
+      </c>
+      <c r="D18" s="4" t="inlineStr">
+        <is>
+          <t>кДж/кг</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="9" t="inlineStr">
+        <is>
+          <t>1.4 Номинальная расход</t>
+        </is>
+      </c>
+      <c r="C20" s="4" t="n"/>
+      <c r="D20" s="4" t="n"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Произведение КПД принемаем:</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="4" t="n"/>
+      <c r="C21" s="4" t="n"/>
+      <c r="D21" s="4" t="n"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>ηoi*ηм*ηг =</t>
+        </is>
+      </c>
+      <c r="H21" s="14" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="22" ht="18" customHeight="1">
+      <c r="B22" s="11" t="inlineStr">
+        <is>
+          <t>G0=</t>
+        </is>
+      </c>
+      <c r="C22" s="12" t="n">
+        <v>230.7382694367192</v>
+      </c>
+      <c r="D22" s="4" t="inlineStr">
+        <is>
+          <t>кг/с</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Находим электрическую мощносчть ЦВД турбины</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Nэ=</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>43172.9009942295</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>кВт</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2. Оценка потель давления в паровпускных органах</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="18" customHeight="1">
+      <c r="B27" s="4" t="inlineStr">
+        <is>
+          <t>Примем ∆p/p0</t>
+        </is>
+      </c>
+      <c r="C27" s="13" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="D27" s="4" t="inlineStr">
+        <is>
+          <t>Следовательно</t>
+        </is>
+      </c>
+      <c r="E27" s="4" t="inlineStr">
+        <is>
+          <t>p0'</t>
+        </is>
+      </c>
+      <c r="F27" s="4" t="n">
+        <v>12.35</v>
+      </c>
+      <c r="G27" s="4" t="inlineStr">
+        <is>
+          <t>МПа</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="n"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>3. Параметры пара после регулирующих клапанов</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="n"/>
+    </row>
+    <row r="31" ht="17.25" customHeight="1">
+      <c r="A31" s="4" t="n"/>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
+          <t>Р, МПа</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="inlineStr">
+        <is>
+          <t>t, oC</t>
+        </is>
+      </c>
+      <c r="D31" s="15" t="inlineStr">
+        <is>
+          <t>h, кДж/кг</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>S, кДж/кг</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>v, м3/кг</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="inlineStr">
+        <is>
+          <t>Индекс 0 (штрих)</t>
+        </is>
+      </c>
+      <c r="B32" s="5">
+        <f>F27</f>
+        <v/>
+      </c>
+      <c r="C32" s="10" t="n">
+        <v>820.4190007152333</v>
+      </c>
+      <c r="D32" s="10" t="n">
+        <v>3470.996181930883</v>
+      </c>
+      <c r="E32" s="7" t="n">
+        <v>6.630048689665621</v>
+      </c>
+      <c r="F32" s="8" t="n">
+        <v>0.02827546851902559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add adding text to the interface
</commit_message>
<xml_diff>
--- a/DB/raschet_turboagregata_predvaritelny.xlsx
+++ b/DB/raschet_turboagregata_predvaritelny.xlsx
@@ -571,30 +571,30 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>ЛМЗ, ЦВД</t>
+          <t>УТЗ, ЦВД</t>
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>550</v>
+        <v>2</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>3.6</v>
+        <v>2</v>
       </c>
       <c r="H3" s="3" t="n"/>
       <c r="I3" s="3" t="n">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>130</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -654,13 +654,13 @@
         <v/>
       </c>
       <c r="D9" s="6" t="n">
-        <v>3470.996181930883</v>
+        <v>8.767939928491167</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>6.608253838576329</v>
+        <v>0.02834233223622572</v>
       </c>
       <c r="F9" s="8" t="n">
-        <v>0.02685306336725179</v>
+        <v>0.0009996105588871713</v>
       </c>
     </row>
     <row r="11">
@@ -709,17 +709,17 @@
         <v/>
       </c>
       <c r="C14" s="10" t="n">
-        <v>341.069773726435</v>
+        <v>1.998035383653871</v>
       </c>
       <c r="D14" s="6" t="n">
-        <v>3080.291195557765</v>
+        <v>9.767300492850904</v>
       </c>
       <c r="E14" s="7">
         <f>E9</f>
         <v/>
       </c>
       <c r="F14" s="8" t="n">
-        <v>0.07308081411324667</v>
+        <v>0.0009991108376305076</v>
       </c>
     </row>
     <row r="16">
@@ -743,7 +743,7 @@
         </is>
       </c>
       <c r="C18" s="4" t="n">
-        <v>390.7049863731177</v>
+        <v>-0.999360564359737</v>
       </c>
       <c r="D18" s="4" t="inlineStr">
         <is>
@@ -785,7 +785,7 @@
         </is>
       </c>
       <c r="C22" s="12" t="n">
-        <v>230.7382694367192</v>
+        <v>-14126.68016159745</v>
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>43172.9009942295</v>
+        <v>28833.51946702796</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="F27" s="4" t="n">
-        <v>12.35</v>
+        <v>0.95</v>
       </c>
       <c r="G27" s="4" t="inlineStr">
         <is>
@@ -900,16 +900,16 @@
         <v/>
       </c>
       <c r="C32" s="10" t="n">
-        <v>820.4190007152333</v>
+        <v>2.011978024246901</v>
       </c>
       <c r="D32" s="10" t="n">
-        <v>3470.996181930883</v>
+        <v>8.767939928491167</v>
       </c>
       <c r="E32" s="7" t="n">
-        <v>6.630048689665621</v>
+        <v>0.02852407789332977</v>
       </c>
       <c r="F32" s="8" t="n">
-        <v>0.02827546851902559</v>
+        <v>0.0009996352088091508</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Output of values to the interface
</commit_message>
<xml_diff>
--- a/DB/raschet_turboagregata_predvaritelny.xlsx
+++ b/DB/raschet_turboagregata_predvaritelny.xlsx
@@ -566,35 +566,35 @@
     <row r="3">
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Т-100-130</t>
+          <t>К-300-23,5</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>УТЗ, ЦВД</t>
+          <t>ЛМЗ, ЦВД</t>
         </is>
       </c>
       <c r="D3" s="3" t="n">
         <v>12</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3" s="3" t="n">
         <v>2</v>
       </c>
       <c r="H3" s="3" t="n"/>
       <c r="I3" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -654,13 +654,13 @@
         <v/>
       </c>
       <c r="D9" s="6" t="n">
-        <v>8.767939928491167</v>
+        <v>13.97868135173841</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>0.02834233223622572</v>
+        <v>0.04362872542254398</v>
       </c>
       <c r="F9" s="8" t="n">
-        <v>0.0009996105588871713</v>
+        <v>0.0009990908150413771</v>
       </c>
     </row>
     <row r="11">
@@ -709,17 +709,17 @@
         <v/>
       </c>
       <c r="C14" s="10" t="n">
-        <v>1.998035383653871</v>
+        <v>2.999999999999773</v>
       </c>
       <c r="D14" s="6" t="n">
-        <v>9.767300492850904</v>
+        <v>13.97868135173728</v>
       </c>
       <c r="E14" s="7">
         <f>E9</f>
         <v/>
       </c>
       <c r="F14" s="8" t="n">
-        <v>0.0009991108376305076</v>
+        <v>0.0009990908150413771</v>
       </c>
     </row>
     <row r="16">
@@ -743,7 +743,7 @@
         </is>
       </c>
       <c r="C18" s="4" t="n">
-        <v>-0.999360564359737</v>
+        <v>1.13509202037676e-12</v>
       </c>
       <c r="D18" s="4" t="inlineStr">
         <is>
@@ -785,7 +785,7 @@
         </is>
       </c>
       <c r="C22" s="12" t="n">
-        <v>-14126.68016159745</v>
+        <v>1.243744718964512e+16</v>
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>28833.51946702796</v>
+        <v>2027.239756462033</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="F27" s="4" t="n">
-        <v>0.95</v>
+        <v>1.9</v>
       </c>
       <c r="G27" s="4" t="inlineStr">
         <is>
@@ -900,16 +900,16 @@
         <v/>
       </c>
       <c r="C32" s="10" t="n">
-        <v>2.011978024246901</v>
+        <v>3.023854003193946</v>
       </c>
       <c r="D32" s="10" t="n">
-        <v>8.767939928491167</v>
+        <v>13.97868135173841</v>
       </c>
       <c r="E32" s="7" t="n">
-        <v>0.02852407789332977</v>
+        <v>0.04399070813284934</v>
       </c>
       <c r="F32" s="8" t="n">
-        <v>0.0009996352088091508</v>
+        <v>0.0009991400950681406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add func HTofRS, SM_CS_ExLos.
add data d_rs.

add if calculation H0_rs.
</commit_message>
<xml_diff>
--- a/DB/raschet_turboagregata_predvaritelny.xlsx
+++ b/DB/raschet_turboagregata_predvaritelny.xlsx
@@ -21,7 +21,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -35,6 +35,15 @@
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <vertAlign val="superscript"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -118,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -160,6 +169,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -507,21 +519,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:K32"/>
+  <dimension ref="A2:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="L41" sqref="K41:L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" ht="18" customHeight="1">
-      <c r="B2" s="15" t="inlineStr">
+      <c r="B2" s="16" t="inlineStr">
         <is>
           <t>Маркировка турбины</t>
         </is>
       </c>
-      <c r="C2" s="16" t="n"/>
+      <c r="C2" s="17" t="n"/>
       <c r="D2" s="2" t="inlineStr">
         <is>
           <t>N, МВт</t>
@@ -566,7 +578,7 @@
     <row r="3">
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>К-300-23,5</t>
+          <t>Т-100-130</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
@@ -575,26 +587,28 @@
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>3</v>
+        <v>550</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="n"/>
+        <v>3.6</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="I3" s="3" t="n">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>3</v>
+        <v>180</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5">
@@ -623,7 +637,7 @@
           <t>t, oC</t>
         </is>
       </c>
-      <c r="D8" s="15" t="inlineStr">
+      <c r="D8" s="16" t="inlineStr">
         <is>
           <t>h, кДж/кг</t>
         </is>
@@ -654,13 +668,13 @@
         <v/>
       </c>
       <c r="D9" s="6" t="n">
-        <v>13.97868135173841</v>
+        <v>3470.996181930883</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>0.04362872542254398</v>
+        <v>6.608253838576329</v>
       </c>
       <c r="F9" s="8" t="n">
-        <v>0.0009990908150413771</v>
+        <v>0.02685306336725179</v>
       </c>
     </row>
     <row r="11">
@@ -682,7 +696,7 @@
           <t>t, oC</t>
         </is>
       </c>
-      <c r="D13" s="15" t="inlineStr">
+      <c r="D13" s="16" t="inlineStr">
         <is>
           <t>h, кДж/кг</t>
         </is>
@@ -709,17 +723,17 @@
         <v/>
       </c>
       <c r="C14" s="10" t="n">
-        <v>2.999999999999773</v>
+        <v>341.069773726435</v>
       </c>
       <c r="D14" s="6" t="n">
-        <v>13.97868135173728</v>
+        <v>3080.291195557765</v>
       </c>
       <c r="E14" s="7">
         <f>E9</f>
         <v/>
       </c>
       <c r="F14" s="8" t="n">
-        <v>0.0009990908150413771</v>
+        <v>0.07308081411324667</v>
       </c>
     </row>
     <row r="16">
@@ -743,7 +757,7 @@
         </is>
       </c>
       <c r="C18" s="4" t="n">
-        <v>1.13509202037676e-12</v>
+        <v>390.7049863731177</v>
       </c>
       <c r="D18" s="4" t="inlineStr">
         <is>
@@ -785,7 +799,7 @@
         </is>
       </c>
       <c r="C22" s="12" t="n">
-        <v>1.243744718964512e+16</v>
+        <v>230.7382694367192</v>
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
@@ -807,7 +821,7 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>2027.239756462033</v>
+        <v>43172.9009942295</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -842,7 +856,7 @@
         </is>
       </c>
       <c r="F27" s="4" t="n">
-        <v>1.9</v>
+        <v>12.35</v>
       </c>
       <c r="G27" s="4" t="inlineStr">
         <is>
@@ -873,7 +887,7 @@
           <t>t, oC</t>
         </is>
       </c>
-      <c r="D31" s="15" t="inlineStr">
+      <c r="D31" s="16" t="inlineStr">
         <is>
           <t>h, кДж/кг</t>
         </is>
@@ -900,16 +914,107 @@
         <v/>
       </c>
       <c r="C32" s="10" t="n">
-        <v>3.023854003193946</v>
+        <v>547.4190007152333</v>
       </c>
       <c r="D32" s="10" t="n">
-        <v>13.97868135173841</v>
+        <v>3470.996181930883</v>
       </c>
       <c r="E32" s="7" t="n">
-        <v>0.04399070813284934</v>
+        <v>6.630048689665621</v>
       </c>
       <c r="F32" s="8" t="n">
-        <v>0.0009991400950681406</v>
+        <v>0.02827546851902559</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>4. Параметры пара на выходе из регулирующей ступени</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>4.1 Параметры пара после регулирующей ступени (без учета потерь)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" s="9" t="inlineStr">
+        <is>
+          <t>4.1.1 Располагаемый теплоперепад рег.ступени</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" ht="18" customHeight="1">
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Отношение скоростей, u/cф=</t>
+        </is>
+      </c>
+      <c r="E37" s="14" t="n">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="38" ht="18.75" customHeight="1">
+      <c r="D38" s="15" t="inlineStr">
+        <is>
+          <t>H0рс, кДж/кг</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" ht="17.25" customHeight="1">
+      <c r="A41" s="4" t="n"/>
+      <c r="B41" s="2" t="inlineStr">
+        <is>
+          <t>Р, МПа</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="inlineStr">
+        <is>
+          <t>t, oC</t>
+        </is>
+      </c>
+      <c r="D41" s="16" t="inlineStr">
+        <is>
+          <t>h, кДж/кг</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>S, кДж/кг</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>v, м3/кг</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="inlineStr">
+        <is>
+          <t>Индекс 2рсt</t>
+        </is>
+      </c>
+      <c r="B42" s="5" t="n">
+        <v>7.148328643637858</v>
+      </c>
+      <c r="C42" s="10" t="n">
+        <v>452.1459474068108</v>
+      </c>
+      <c r="D42" s="10" t="n">
+        <v>3290.996181930883</v>
+      </c>
+      <c r="E42" s="7" t="n">
+        <v>6.630048689665621</v>
+      </c>
+      <c r="F42" s="8" t="n">
+        <v>0.0433555151468901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>